<commit_message>
Fixing issue only in English
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2044B4CA-ED8A-4995-A258-ABF7E0456969}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A84931-F6E9-452B-AF14-310DFF4F848D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="112">
   <si>
     <t>,</t>
   </si>
@@ -722,9 +722,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2036,9 +2036,7 @@
         <v>22</v>
       </c>
       <c r="C64" s="1"/>
-      <c r="D64" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D64" s="1"/>
       <c r="E64" s="1" t="s">
         <v>108</v>
       </c>
@@ -2299,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD67DD9-13C8-46B0-8ACB-1FB3870C0C69}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed edition in English JIDS
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A84931-F6E9-452B-AF14-310DFF4F848D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF92EB1-E1E8-484F-8F59-E066C0EFA8E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="114">
   <si>
     <t>,</t>
   </si>
@@ -357,6 +357,12 @@
   </si>
   <si>
     <t>a-page-range-delimiter</t>
+  </si>
+  <si>
+    <t>b-secondary-contributor-label-right</t>
+  </si>
+  <si>
+    <t>b-secondary-contributor-label-left</t>
   </si>
 </sst>
 </file>
@@ -720,11 +726,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L76"/>
+  <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1296,14 +1302,12 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1312,16 +1316,16 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="D28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -1331,42 +1335,30 @@
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C29" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>0</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
         <v>19</v>
       </c>
@@ -1379,41 +1371,41 @@
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
+      <c r="A31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>19</v>
@@ -1426,14 +1418,22 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -1442,56 +1442,62 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B36" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C36" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D36" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E36" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-    </row>
-    <row r="35" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-    </row>
-    <row r="36" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
@@ -1502,16 +1508,16 @@
     </row>
     <row r="37" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E37" s="5"/>
+        <v>63</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="9"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -1521,17 +1527,11 @@
       <c r="L37" s="9"/>
     </row>
     <row r="38" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E38" s="5"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="39" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>51</v>
@@ -1562,20 +1562,16 @@
     </row>
     <row r="40" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="C40" s="5"/>
       <c r="D40" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E40" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="E40" s="5"/>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
@@ -1585,11 +1581,17 @@
       <c r="L40" s="9"/>
     </row>
     <row r="41" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
+      <c r="A41" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" s="5"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -1598,18 +1600,22 @@
       <c r="K41" s="9"/>
       <c r="L41" s="9"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="9"/>
+        <v>73</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
@@ -1618,62 +1624,52 @@
       <c r="K42" s="9"/>
       <c r="L42" s="9"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
+    <row r="43" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
+      <c r="A44" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E45" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -1684,19 +1680,19 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -1707,10 +1703,16 @@
       <c r="L46" s="1"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
+      <c r="A47" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
+      <c r="D47" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -1722,12 +1724,16 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D48" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>19</v>
@@ -1741,9 +1747,7 @@
       <c r="L48" s="1"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1757,11 +1761,17 @@
       <c r="L49" s="1"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
+      <c r="A50" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -1772,20 +1782,12 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -1795,21 +1797,11 @@
       <c r="L51" s="1"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>19</v>
-      </c>
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -1820,19 +1812,19 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B53" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C53" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D53" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E53" s="1" t="b">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -1844,12 +1836,20 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>19</v>
+      </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -1860,15 +1860,19 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1" t="s">
-        <v>19</v>
+        <v>47</v>
+      </c>
+      <c r="B55" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C55" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D55" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -1880,20 +1884,12 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C56" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D56" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" s="1" t="b">
-        <v>1</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -1904,17 +1900,15 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D57" s="1"/>
       <c r="E57" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -1926,14 +1920,20 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E58" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="B58" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C58" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D58" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
@@ -1944,16 +1944,18 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="D59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E59" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -1964,7 +1966,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1981,10 +1983,16 @@
       <c r="L60" s="1"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
+      <c r="A61" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
+      <c r="D61" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -1995,15 +2003,15 @@
       <c r="L61" s="1"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62" s="11" t="s">
-        <v>54</v>
+      <c r="A62" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1" t="s">
-        <v>108</v>
-      </c>
+      <c r="D62" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -2013,9 +2021,7 @@
       <c r="L62" s="1"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63" s="11" t="s">
-        <v>55</v>
-      </c>
+      <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -2030,11 +2036,9 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1" t="s">
@@ -2050,11 +2054,9 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -2068,15 +2070,15 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B66" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D66" s="1"/>
       <c r="E66" s="1" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -2087,8 +2089,12 @@
       <c r="L66" s="1"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A67" s="11"/>
-      <c r="B67" s="1"/>
+      <c r="A67" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -2102,19 +2108,15 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B68" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="E68" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -2125,21 +2127,11 @@
       <c r="L68" s="1"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A69" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="A69" s="11"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
@@ -2149,11 +2141,21 @@
       <c r="L69" s="1"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
+      <c r="A70" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
@@ -2163,20 +2165,20 @@
       <c r="L70" s="1"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B71" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C71" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D71" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E71" s="1" t="b">
-        <v>1</v>
+      <c r="A71" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -2202,16 +2204,20 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E73" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="B73" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C73" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D73" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
@@ -2221,16 +2227,10 @@
       <c r="L73" s="1"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A74" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -2241,21 +2241,17 @@
       <c r="L74" s="1"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A75" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B75" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C75" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D75" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E75" s="1" t="b">
-        <v>0</v>
-      </c>
+      <c r="A75" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
@@ -2266,20 +2262,16 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
@@ -2287,6 +2279,54 @@
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A77" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B77" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C77" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D77" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A78" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tested all Japanese styles
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB58455-D473-42A7-9C00-EB49DBAC9394}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24F64FD-51A8-4402-81DE-EE5DD9BF6529}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="145">
   <si>
     <t>,</t>
   </si>
@@ -212,9 +212,6 @@
     <t>b-journal-title-right</t>
   </si>
   <si>
-    <t>b-book-authors-suffix</t>
-  </si>
-  <si>
     <t>b-article-page-label-invert</t>
   </si>
   <si>
@@ -399,6 +396,66 @@
   </si>
   <si>
     <t>b-name-part-delimiter</t>
+  </si>
+  <si>
+    <t>b-publisher-remove-place</t>
+  </si>
+  <si>
+    <t>b-locators-chapter-after-issue</t>
+  </si>
+  <si>
+    <t>b-locator-chapter-suffix</t>
+  </si>
+  <si>
+    <t>b-accessed-left</t>
+  </si>
+  <si>
+    <t>b-accessed-right</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> アクセス）</t>
+  </si>
+  <si>
+    <t>b-accessed-format</t>
+  </si>
+  <si>
+    <t>yyyy/mm/dd</t>
+  </si>
+  <si>
+    <t>c-locator-label-form</t>
+  </si>
+  <si>
+    <t>c-locator-label-right</t>
+  </si>
+  <si>
+    <t>webpage</t>
+  </si>
+  <si>
+    <t>b-final-punctuation-omit-type</t>
+  </si>
+  <si>
+    <t>b-edition-left</t>
+  </si>
+  <si>
+    <t>b-publisher-group-left</t>
+  </si>
+  <si>
+    <t>b-publisher-group-right</t>
+  </si>
+  <si>
+    <t>b-translator-editor</t>
+  </si>
+  <si>
+    <t>b-translator-editor-delimiter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> アクセス) </t>
+  </si>
+  <si>
+    <t>b-url-left</t>
+  </si>
+  <si>
+    <t>b-doi-left</t>
   </si>
 </sst>
 </file>
@@ -422,7 +479,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -445,11 +502,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -482,11 +552,46 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -773,11 +878,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L85"/>
+  <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L52" sqref="L52"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,6 +892,7 @@
     <col min="3" max="3" width="9" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -794,24 +900,24 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="F1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="16"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -819,7 +925,7 @@
     </row>
     <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>44</v>
@@ -839,7 +945,7 @@
       <c r="G2" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="13"/>
+      <c r="H2" s="17"/>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
@@ -847,7 +953,7 @@
     </row>
     <row r="3" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>51</v>
@@ -867,7 +973,7 @@
       <c r="G3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="18"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -875,7 +981,7 @@
     </row>
     <row r="4" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>23</v>
@@ -895,7 +1001,7 @@
       <c r="G4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="5"/>
+      <c r="H4" s="18"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -903,27 +1009,27 @@
     </row>
     <row r="5" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="H5" s="9"/>
+        <v>109</v>
+      </c>
+      <c r="H5" s="19"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
@@ -931,7 +1037,7 @@
     </row>
     <row r="6" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>34</v>
@@ -946,12 +1052,12 @@
         <v>34</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="H6" s="9"/>
+        <v>118</v>
+      </c>
+      <c r="H6" s="19"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -979,7 +1085,7 @@
       <c r="G7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="5"/>
+      <c r="H7" s="18"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -1007,7 +1113,7 @@
       <c r="G8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="3"/>
+      <c r="H8" s="20"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1021,19 +1127,19 @@
         <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="H9" s="3"/>
+        <v>92</v>
+      </c>
+      <c r="H9" s="20"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1061,7 +1167,7 @@
       <c r="G10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="21"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1069,7 +1175,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B11" s="1" t="b">
         <v>0</v>
@@ -1089,7 +1195,7 @@
       <c r="G11" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="21"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1097,7 +1203,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B12" s="1" t="b">
         <v>0</v>
@@ -1117,7 +1223,7 @@
       <c r="G12" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="21"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1139,7 +1245,7 @@
         <v>37</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="H13" s="21"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1161,11 +1267,9 @@
       <c r="E14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="21"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1173,107 +1277,101 @@
     </row>
     <row r="15" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="21"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>134</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="21"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="A18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="22"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="H19" s="21"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -1281,39 +1379,41 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="21"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>125</v>
-      </c>
+      <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -1321,155 +1421,141 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>1</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>1</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H22" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="21"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H23" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="H23" s="21"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="21"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D25" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E25" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="F25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="21"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
+      <c r="A26" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" s="19"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>82</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="H27" s="21"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -1477,15 +1563,27 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" s="21"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -1493,21 +1591,23 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="D29" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="H29" s="21"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -1515,17 +1615,15 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
+      <c r="H30" s="21"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -1533,15 +1631,21 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B31" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="F31" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="H31" s="21"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -1549,15 +1653,17 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="H32" s="21"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -1565,17 +1671,15 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="H33" s="21"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -1583,249 +1687,241 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="H34" s="21"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="D35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="H35" s="21"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C36" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D36" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E36" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G36" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+    </row>
+    <row r="37" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" s="1"/>
+        <v>104</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G37" s="9"/>
+      <c r="H37" s="21"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
+      <c r="A38" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" s="20"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H39" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="H39" s="21"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H40" s="21"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
     </row>
-    <row r="41" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+    </row>
+    <row r="42" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+    </row>
+    <row r="43" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B43" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C43" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D43" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E43" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="F43" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="G43" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-    </row>
-    <row r="42" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
-    </row>
-    <row r="43" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
+      <c r="H43" s="19"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
       <c r="L43" s="9"/>
     </row>
     <row r="44" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G44" s="5"/>
-      <c r="H44" s="9"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="19"/>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
@@ -1833,21 +1929,21 @@
     </row>
     <row r="45" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="G45" s="5"/>
-      <c r="H45" s="9"/>
+      <c r="H45" s="19"/>
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
@@ -1855,21 +1951,21 @@
     </row>
     <row r="46" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="G46" s="5"/>
-      <c r="H46" s="9"/>
+      <c r="H46" s="19"/>
       <c r="I46" s="9"/>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
@@ -1877,113 +1973,107 @@
     </row>
     <row r="47" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C47" s="5"/>
       <c r="D47" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="E47" s="5"/>
       <c r="F47" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H47" s="9"/>
+        <v>51</v>
+      </c>
+      <c r="G47" s="5"/>
+      <c r="H47" s="19"/>
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
     </row>
     <row r="48" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
+      <c r="A48" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H48" s="19"/>
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>34</v>
-      </c>
+    <row r="49" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
       <c r="C49" s="9"/>
-      <c r="D49" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="D49" s="9"/>
       <c r="E49" s="9"/>
-      <c r="F49" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="F49" s="9"/>
       <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
+      <c r="H49" s="19"/>
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
+      <c r="A50" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G50" s="9"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H51" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="H51" s="21"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
@@ -1991,21 +2081,25 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C52" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="D52" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H52" s="21"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
@@ -2013,61 +2107,63 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H53" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="G53" s="1"/>
+      <c r="H53" s="21"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
+      <c r="A54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H54" s="21"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
+      <c r="H55" s="21"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
@@ -2075,57 +2171,49 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
+      <c r="D56" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
+      <c r="H56" s="21"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
+      <c r="A57" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
+      <c r="H57" s="21"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H58" s="1"/>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="21"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
@@ -2133,27 +2221,27 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E59" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F59" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G59" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H59" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H59" s="21"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
@@ -2161,27 +2249,25 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B60" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C60" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D60" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G60" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H60" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G60" s="11"/>
+      <c r="H60" s="21"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
@@ -2189,15 +2275,17 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H61" s="21"/>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
@@ -2205,21 +2293,27 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H62" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="B62" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C62" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D62" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H62" s="21"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
@@ -2227,27 +2321,19 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B63" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C63" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D63" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G63" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H63" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H63" s="21"/>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
@@ -2255,21 +2341,23 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D64" s="1"/>
       <c r="E64" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H64" s="21"/>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
@@ -2277,17 +2365,27 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="B65" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C65" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D65" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G65" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H65" s="21"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
@@ -2295,21 +2393,21 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C66" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="D66" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F66" s="1"/>
       <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
+      <c r="H66" s="21"/>
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
@@ -2317,65 +2415,69 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
+      <c r="H67" s="21"/>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
+      <c r="A68" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
+      <c r="D68" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
+      <c r="H68" s="21"/>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
-        <v>54</v>
+      <c r="A69" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1" t="s">
-        <v>108</v>
-      </c>
+      <c r="D69" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
+      <c r="H69" s="21"/>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
-        <v>55</v>
-      </c>
+      <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
+      <c r="H70" s="21"/>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
@@ -2383,23 +2485,17 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H71" s="1"/>
+        <v>107</v>
+      </c>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="21"/>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
@@ -2407,21 +2503,15 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
-      <c r="F72" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="21"/>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
@@ -2429,7 +2519,7 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>22</v>
@@ -2437,11 +2527,15 @@
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
+        <v>107</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H73" s="21"/>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
@@ -2449,7 +2543,7 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
-        <v>123</v>
+        <v>57</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>23</v>
@@ -2457,9 +2551,13 @@
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
+      <c r="F74" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H74" s="21"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
@@ -2467,33 +2565,37 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B75" s="1"/>
+        <v>121</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C75" s="1"/>
-      <c r="D75" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D75" s="1"/>
       <c r="E75" s="1" t="s">
-        <v>19</v>
+        <v>107</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
+      <c r="H75" s="21"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" s="11"/>
-      <c r="B76" s="1"/>
+      <c r="A76" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
+      <c r="H76" s="21"/>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
@@ -2501,97 +2603,89 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B77" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="E77" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H77" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="21"/>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H78" s="1"/>
+      <c r="A78" s="11"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="21"/>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
+      <c r="A79" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H79" s="21"/>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B80" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C80" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D80" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F80" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G80" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H80" s="1"/>
+      <c r="A80" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H80" s="21"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
@@ -2605,7 +2699,7 @@
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
+      <c r="H81" s="21"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
@@ -2613,109 +2707,432 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="B82" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C82" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D82" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G82" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H82" s="21"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A83" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="D83" s="1"/>
       <c r="E83" s="1"/>
-      <c r="F83" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="F83" s="1"/>
       <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
+      <c r="H83" s="21"/>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
       <c r="L83" s="1"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B84" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C84" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D84" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F84" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G84" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H84" s="1"/>
+      <c r="A84" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H84" s="21"/>
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" s="11" t="s">
-        <v>107</v>
+      <c r="A85" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="C85" s="1"/>
       <c r="D85" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E85" s="1" t="s">
-        <v>106</v>
-      </c>
+      <c r="E85" s="1"/>
       <c r="F85" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H85" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="H85" s="21"/>
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
     </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H86" s="21"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+      <c r="L86" s="1"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H87" s="21"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="1"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H88" s="21"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+      <c r="K88" s="1"/>
+      <c r="L88" s="1"/>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G89" s="1"/>
+      <c r="H89" s="21"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+      <c r="K89" s="1"/>
+      <c r="L89" s="1"/>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B90" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C90" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D90" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F90" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G90" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H90" s="21"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+      <c r="K90" s="1"/>
+      <c r="L90" s="1"/>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H91" s="21"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="1"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H92" s="21"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G93" s="1"/>
+      <c r="H93" s="21"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+      <c r="L93" s="1"/>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="21"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B95" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C95" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D95" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F95" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G95" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H95" s="21"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G96" s="1"/>
+      <c r="H96" s="21"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+      <c r="L96" s="1"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="11"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="21"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+      <c r="L97" s="1"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B98" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C98" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D98" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G98" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H98" s="21"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+      <c r="L98" s="1"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B99" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C99" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D99" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E99" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F99" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G99" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:G1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>" "</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2741,7 +3158,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>49</v>
@@ -2750,27 +3167,27 @@
         <v>50</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>95</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -2781,16 +3198,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>
@@ -2801,16 +3218,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -2821,16 +3238,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" t="s">
         <v>22</v>
@@ -2841,16 +3258,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -2861,16 +3278,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Adding indent to kyoso-ja -en
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51DC809-2548-494F-B7C1-95E94ADC11ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE94B2C-D665-41C9-B3E5-B1534D7B14D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="180">
   <si>
     <t>,</t>
   </si>
@@ -556,19 +556,30 @@
   </si>
   <si>
     <t>b-secondary-contributor-initialize</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>b-access-display-newline</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -619,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -655,11 +666,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="11">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -667,106 +679,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1146,28 +1058,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L110"/>
+  <dimension ref="A1:L111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J59" sqref="J59"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1203,7 +1115,7 @@
       </c>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="14" customFormat="1">
       <c r="A2" s="13" t="s">
         <v>91</v>
       </c>
@@ -1239,7 +1151,7 @@
       </c>
       <c r="L2" s="13"/>
     </row>
-    <row r="3" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="6" customFormat="1">
       <c r="A3" s="5" t="s">
         <v>67</v>
       </c>
@@ -1275,7 +1187,7 @@
       </c>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="6" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>68</v>
       </c>
@@ -1311,7 +1223,7 @@
       </c>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="15" customFormat="1">
       <c r="A5" s="9" t="s">
         <v>110</v>
       </c>
@@ -1347,7 +1259,7 @@
       </c>
       <c r="L5" s="9"/>
     </row>
-    <row r="6" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" s="15" customFormat="1">
       <c r="A6" s="9" t="s">
         <v>151</v>
       </c>
@@ -1367,7 +1279,7 @@
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="15" customFormat="1">
       <c r="A7" s="9" t="s">
         <v>117</v>
       </c>
@@ -1403,7 +1315,7 @@
       </c>
       <c r="L7" s="9"/>
     </row>
-    <row r="8" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="4" customFormat="1">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
@@ -1439,7 +1351,7 @@
       </c>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="4" customFormat="1">
       <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
@@ -1475,7 +1387,7 @@
       </c>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12">
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
@@ -1511,7 +1423,7 @@
       </c>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1547,7 +1459,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>120</v>
       </c>
@@ -1583,7 +1495,7 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
         <v>119</v>
       </c>
@@ -1619,7 +1531,7 @@
       </c>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1647,7 +1559,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" s="8" customFormat="1">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1671,7 +1583,7 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" s="8" customFormat="1">
       <c r="A16" s="1" t="s">
         <v>123</v>
       </c>
@@ -1697,7 +1609,7 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" s="8" customFormat="1">
       <c r="A17" s="1" t="s">
         <v>133</v>
       </c>
@@ -1719,7 +1631,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" s="8" customFormat="1">
       <c r="A18" s="1" t="s">
         <v>134</v>
       </c>
@@ -1741,7 +1653,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12">
       <c r="A19" s="7" t="s">
         <v>5</v>
       </c>
@@ -1777,7 +1689,7 @@
       </c>
       <c r="L19" s="7"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -1793,7 +1705,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -1829,7 +1741,7 @@
       </c>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1843,7 +1755,7 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
         <v>171</v>
       </c>
@@ -1879,7 +1791,7 @@
       </c>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -1899,7 +1811,7 @@
       </c>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12">
       <c r="A25" s="1" t="s">
         <v>11</v>
       </c>
@@ -1922,12 +1834,12 @@
         <v>37</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>37</v>
+        <v>178</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12">
       <c r="A26" s="1" t="s">
         <v>124</v>
       </c>
@@ -1947,7 +1859,7 @@
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
@@ -1983,7 +1895,7 @@
       </c>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" s="10" customFormat="1">
       <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
@@ -2019,7 +1931,7 @@
       </c>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12">
       <c r="A29" s="9" t="s">
         <v>100</v>
       </c>
@@ -2053,7 +1965,7 @@
       </c>
       <c r="L29" s="9"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
@@ -2077,7 +1989,7 @@
       </c>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12">
       <c r="A31" s="1" t="s">
         <v>176</v>
       </c>
@@ -2111,7 +2023,7 @@
       </c>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12">
       <c r="A32" s="1" t="s">
         <v>174</v>
       </c>
@@ -2135,7 +2047,7 @@
       </c>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12">
       <c r="A33" s="1" t="s">
         <v>177</v>
       </c>
@@ -2169,7 +2081,7 @@
       </c>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12">
       <c r="A34" s="1" t="s">
         <v>175</v>
       </c>
@@ -2189,7 +2101,7 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12">
       <c r="A35" s="1" t="s">
         <v>15</v>
       </c>
@@ -2225,7 +2137,7 @@
       </c>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12">
       <c r="A36" s="1" t="s">
         <v>82</v>
       </c>
@@ -2255,7 +2167,7 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12">
       <c r="A37" s="1" t="s">
         <v>83</v>
       </c>
@@ -2273,7 +2185,7 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12">
       <c r="A38" s="1" t="s">
         <v>84</v>
       </c>
@@ -2299,7 +2211,7 @@
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12">
       <c r="A39" s="1" t="s">
         <v>101</v>
       </c>
@@ -2317,7 +2229,7 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12">
       <c r="A40" s="1" t="s">
         <v>102</v>
       </c>
@@ -2333,7 +2245,7 @@
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12">
       <c r="A41" s="1" t="s">
         <v>112</v>
       </c>
@@ -2349,7 +2261,7 @@
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12">
       <c r="A42" s="1" t="s">
         <v>111</v>
       </c>
@@ -2367,7 +2279,7 @@
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12">
       <c r="A43" s="1" t="s">
         <v>103</v>
       </c>
@@ -2385,7 +2297,7 @@
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
     </row>
-    <row r="44" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" s="4" customFormat="1">
       <c r="A44" s="1" t="s">
         <v>104</v>
       </c>
@@ -2411,7 +2323,7 @@
       <c r="K44" s="9"/>
       <c r="L44" s="1"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12">
       <c r="A45" s="3" t="s">
         <v>17</v>
       </c>
@@ -2447,7 +2359,7 @@
       </c>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12">
       <c r="A46" s="1" t="s">
         <v>18</v>
       </c>
@@ -2483,7 +2395,7 @@
       </c>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12">
       <c r="A47" s="1" t="s">
         <v>20</v>
       </c>
@@ -2517,7 +2429,7 @@
       </c>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12">
       <c r="A48" s="1" t="s">
         <v>21</v>
       </c>
@@ -2546,12 +2458,10 @@
       <c r="J48" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="K48" s="1" t="s">
-        <v>173</v>
-      </c>
+      <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" s="10" customFormat="1">
       <c r="A49" s="1" t="s">
         <v>26</v>
       </c>
@@ -2567,7 +2477,7 @@
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" s="10" customFormat="1">
       <c r="A50" s="9" t="s">
         <v>42</v>
       </c>
@@ -2603,7 +2513,7 @@
       </c>
       <c r="L50" s="9"/>
     </row>
-    <row r="51" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" s="10" customFormat="1">
       <c r="A51" s="9"/>
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
@@ -2617,7 +2527,7 @@
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
     </row>
-    <row r="52" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" s="10" customFormat="1">
       <c r="A52" s="9" t="s">
         <v>69</v>
       </c>
@@ -2643,7 +2553,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="9"/>
     </row>
-    <row r="53" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" s="10" customFormat="1">
       <c r="A53" s="9" t="s">
         <v>70</v>
       </c>
@@ -2669,7 +2579,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="9"/>
     </row>
-    <row r="54" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" s="10" customFormat="1">
       <c r="A54" s="9" t="s">
         <v>71</v>
       </c>
@@ -2695,7 +2605,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="9"/>
     </row>
-    <row r="55" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" s="10" customFormat="1">
       <c r="A55" s="9" t="s">
         <v>72</v>
       </c>
@@ -2731,7 +2641,7 @@
       </c>
       <c r="L55" s="9"/>
     </row>
-    <row r="56" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" s="10" customFormat="1">
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
@@ -2745,7 +2655,7 @@
       <c r="K56" s="9"/>
       <c r="L56" s="9"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12">
       <c r="A57" s="9" t="s">
         <v>53</v>
       </c>
@@ -2771,7 +2681,7 @@
       <c r="K57" s="9"/>
       <c r="L57" s="9"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12">
       <c r="A58" s="1" t="s">
         <v>27</v>
       </c>
@@ -2797,7 +2707,7 @@
       </c>
       <c r="L58" s="1"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12">
       <c r="A59" s="1" t="s">
         <v>28</v>
       </c>
@@ -2827,7 +2737,7 @@
       </c>
       <c r="L59" s="1"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12">
       <c r="A60" s="1" t="s">
         <v>31</v>
       </c>
@@ -2851,7 +2761,7 @@
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12">
       <c r="A61" s="1" t="s">
         <v>33</v>
       </c>
@@ -2887,7 +2797,7 @@
       </c>
       <c r="L61" s="1"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2901,7 +2811,7 @@
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12">
       <c r="A63" s="1" t="s">
         <v>96</v>
       </c>
@@ -2921,7 +2831,7 @@
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12">
       <c r="A64" s="1" t="s">
         <v>97</v>
       </c>
@@ -2937,7 +2847,7 @@
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2951,7 +2861,7 @@
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12">
       <c r="A66" s="1" t="s">
         <v>45</v>
       </c>
@@ -2987,7 +2897,7 @@
       </c>
       <c r="L66" s="1"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12">
       <c r="A67" s="1" t="s">
         <v>46</v>
       </c>
@@ -3019,7 +2929,7 @@
       <c r="K67" s="11"/>
       <c r="L67" s="1"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12">
       <c r="A68" s="1" t="s">
         <v>127</v>
       </c>
@@ -3039,7 +2949,7 @@
       </c>
       <c r="L68" s="1"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12">
       <c r="A69" s="1" t="s">
         <v>47</v>
       </c>
@@ -3075,7 +2985,7 @@
       </c>
       <c r="L69" s="1"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12">
       <c r="A70" s="1" t="s">
         <v>48</v>
       </c>
@@ -3097,7 +3007,7 @@
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12">
       <c r="A71" s="1" t="s">
         <v>60</v>
       </c>
@@ -3129,7 +3039,7 @@
       </c>
       <c r="L71" s="1"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12">
       <c r="A72" s="1" t="s">
         <v>58</v>
       </c>
@@ -3165,7 +3075,7 @@
       </c>
       <c r="L72" s="1"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12">
       <c r="A73" s="1" t="s">
         <v>59</v>
       </c>
@@ -3187,7 +3097,7 @@
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12">
       <c r="A74" s="1" t="s">
         <v>64</v>
       </c>
@@ -3205,7 +3115,7 @@
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12">
       <c r="A75" s="1" t="s">
         <v>65</v>
       </c>
@@ -3225,7 +3135,7 @@
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12">
       <c r="A76" s="1" t="s">
         <v>93</v>
       </c>
@@ -3243,7 +3153,7 @@
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3257,7 +3167,7 @@
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12">
       <c r="A78" s="11" t="s">
         <v>54</v>
       </c>
@@ -3275,7 +3185,7 @@
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12">
       <c r="A79" s="11" t="s">
         <v>55</v>
       </c>
@@ -3291,7 +3201,7 @@
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12">
       <c r="A80" s="11" t="s">
         <v>56</v>
       </c>
@@ -3323,7 +3233,7 @@
       </c>
       <c r="L80" s="1"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12">
       <c r="A81" s="11" t="s">
         <v>57</v>
       </c>
@@ -3353,7 +3263,7 @@
       </c>
       <c r="L81" s="1"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12">
       <c r="A82" s="11" t="s">
         <v>121</v>
       </c>
@@ -3373,7 +3283,7 @@
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12">
       <c r="A83" s="11" t="s">
         <v>122</v>
       </c>
@@ -3391,7 +3301,7 @@
       <c r="K83" s="1"/>
       <c r="L83" s="1"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12">
       <c r="A84" s="11" t="s">
         <v>108</v>
       </c>
@@ -3411,7 +3321,7 @@
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12">
       <c r="A85" s="11"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3425,7 +3335,7 @@
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12">
       <c r="A86" s="11" t="s">
         <v>61</v>
       </c>
@@ -3454,14 +3364,14 @@
         <v>29</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="K86" s="1" t="s">
         <v>29</v>
       </c>
       <c r="L86" s="1"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12">
       <c r="A87" s="11" t="s">
         <v>62</v>
       </c>
@@ -3497,7 +3407,7 @@
       </c>
       <c r="L87" s="1"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3511,7 +3421,7 @@
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12">
       <c r="A89" s="1" t="s">
         <v>63</v>
       </c>
@@ -3547,7 +3457,7 @@
       </c>
       <c r="L89" s="1"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3561,7 +3471,7 @@
       <c r="K90" s="1"/>
       <c r="L90" s="1"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12">
       <c r="A91" s="1" t="s">
         <v>137</v>
       </c>
@@ -3589,7 +3499,7 @@
       </c>
       <c r="L91" s="1"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12">
       <c r="A92" s="1" t="s">
         <v>66</v>
       </c>
@@ -3621,7 +3531,7 @@
       </c>
       <c r="L92" s="1"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12">
       <c r="A93" s="1" t="s">
         <v>131</v>
       </c>
@@ -3647,7 +3557,7 @@
       </c>
       <c r="L93" s="1"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12">
       <c r="A94" s="1" t="s">
         <v>157</v>
       </c>
@@ -3673,7 +3583,7 @@
       </c>
       <c r="L94" s="1"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12">
       <c r="A95" s="1" t="s">
         <v>128</v>
       </c>
@@ -3709,7 +3619,7 @@
       </c>
       <c r="L95" s="1"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12">
       <c r="A96" s="1" t="s">
         <v>159</v>
       </c>
@@ -3745,7 +3655,7 @@
       </c>
       <c r="L96" s="1"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12">
       <c r="A97" s="1" t="s">
         <v>129</v>
       </c>
@@ -3781,7 +3691,7 @@
       </c>
       <c r="L97" s="1"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12">
       <c r="A98" s="1" t="s">
         <v>156</v>
       </c>
@@ -3803,7 +3713,7 @@
       <c r="K98" s="1"/>
       <c r="L98" s="1"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12">
       <c r="A99" s="11" t="s">
         <v>73</v>
       </c>
@@ -3829,7 +3739,7 @@
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12">
       <c r="A100" s="11" t="s">
         <v>99</v>
       </c>
@@ -3865,7 +3775,7 @@
       </c>
       <c r="L100" s="1"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12">
       <c r="A101" s="11" t="s">
         <v>106</v>
       </c>
@@ -3901,7 +3811,7 @@
       </c>
       <c r="L101" s="1"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12">
       <c r="A102" s="11" t="s">
         <v>136</v>
       </c>
@@ -3929,7 +3839,7 @@
       </c>
       <c r="L102" s="1"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12">
       <c r="A103" s="11" t="s">
         <v>142</v>
       </c>
@@ -3946,12 +3856,14 @@
       </c>
       <c r="I103" s="1"/>
       <c r="J103" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K103" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="K103" s="17" t="s">
+        <v>92</v>
+      </c>
       <c r="L103" s="1"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12">
       <c r="A104" s="11" t="s">
         <v>143</v>
       </c>
@@ -3967,174 +3879,212 @@
       <c r="K104" s="1"/>
       <c r="L104" s="1"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12">
       <c r="A105" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B105" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C105" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D105" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F105" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G105" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H105" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I105" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J105" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K105" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="L105" s="1"/>
+    </row>
+    <row r="106" spans="1:12">
+      <c r="A106" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B105" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C105" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D105" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E105" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F105" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="G105" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H105" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="I105" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J105" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="K105" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="L105" s="1"/>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A106" s="11" t="s">
+      <c r="B106" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C106" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D106" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F106" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G106" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H106" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I106" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J106" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K106" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L106" s="1"/>
+    </row>
+    <row r="107" spans="1:12">
+      <c r="A107" s="11" t="s">
         <v>138</v>
-      </c>
-      <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
-      <c r="E106" s="1"/>
-      <c r="F106" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G106" s="1"/>
-      <c r="H106" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I106" s="1"/>
-      <c r="J106" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="K106" s="1"/>
-      <c r="L106" s="1"/>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A107" s="11" t="s">
-        <v>139</v>
       </c>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
-      <c r="F107" s="11"/>
+      <c r="F107" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="G107" s="1"/>
-      <c r="H107" s="11"/>
+      <c r="H107" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="I107" s="1"/>
-      <c r="J107" s="11"/>
+      <c r="J107" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="K107" s="1"/>
       <c r="L107" s="1"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12">
       <c r="A108" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="11"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="11"/>
+      <c r="I108" s="1"/>
+      <c r="J108" s="11"/>
+      <c r="K108" s="1"/>
+      <c r="L108" s="1"/>
+    </row>
+    <row r="109" spans="1:12">
+      <c r="A109" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B108" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C108" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D108" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E108" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F108" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="G108" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H108" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="I108" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J108" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="K108" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="L108" s="1"/>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A109" s="11" t="s">
+      <c r="B109" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C109" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D109" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E109" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F109" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G109" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H109" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I109" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J109" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K109" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="L109" s="1"/>
+    </row>
+    <row r="110" spans="1:12">
+      <c r="A110" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B109" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C109" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D109" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E109" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F109" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G109" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H109" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I109" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J109" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K109" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A110" s="11" t="s">
+      <c r="B110" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C110" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D110" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E110" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F110" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G110" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H110" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I110" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J110" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K110" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="L110" s="1"/>
+    </row>
+    <row r="111" spans="1:12">
+      <c r="A111" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B110" s="1"/>
-      <c r="C110" s="1"/>
-      <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
-      <c r="F110" s="1"/>
-      <c r="G110" s="1" t="s">
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H110" s="1"/>
-      <c r="I110" s="1" t="s">
+      <c r="H111" s="1"/>
+      <c r="I111" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J110" s="1"/>
-      <c r="K110" s="1" t="s">
+      <c r="J111" s="1"/>
+      <c r="K111" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="L111" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:G23 F98:I98 B97:G1048576 B23:I23 B25:G95">
+  <conditionalFormatting sqref="B1:G23 F98:I98 B97:G1048576 B23:I23 B25:G95 B105:L105">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>" "</formula>
     </cfRule>
@@ -4142,7 +4092,7 @@
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:I23 H97:I110 H25:I95">
+  <conditionalFormatting sqref="H2:I23 H97:I111 H25:I95">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>" "</formula>
     </cfRule>
@@ -4157,7 +4107,7 @@
       <formula>" "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:K23 J97:K110 J25:K95">
+  <conditionalFormatting sqref="J1:K23 J97:K102 J25:K95 J104:K111 J103">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>" "</formula>
     </cfRule>
@@ -4182,12 +4132,13 @@
       <formula>" "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:L1048576">
+  <conditionalFormatting sqref="A1:L102 A104:L1048576 A103:J103 L103">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"　"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4199,18 +4150,18 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="72.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="72.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="12" t="s">
         <v>79</v>
       </c>
@@ -4233,7 +4184,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -4253,7 +4204,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -4273,7 +4224,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -4293,7 +4244,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -4313,7 +4264,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -4333,7 +4284,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>115</v>
       </c>
@@ -4353,7 +4304,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>149</v>
       </c>
@@ -4373,7 +4324,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>146</v>
       </c>
@@ -4393,7 +4344,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>166</v>
       </c>
@@ -4416,7 +4367,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>161</v>
       </c>
@@ -4451,13 +4402,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>167</v>
       </c>
@@ -4465,7 +4416,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>168</v>
       </c>

</xml_diff>